<commit_message>
Generated output file from workflow
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,7 +546,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ATT01 &amp; COMDC - Not yet responded</t>
+          <t>ATT01 - Not yet responded</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>21 days, 17:23:45.788851</t>
+          <t>21 days, 12:40:50.887174</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>ATT01 &amp; COMDC - Not yet responded</t>
+          <t>ATT01 - Not yet responded</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -613,19 +613,19 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>21 days, 17:23:45.788803</t>
+          <t>21 days, 12:40:50.887103</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EMERGENCY CREW EN ROUTE, ETA BY -5:00PM</t>
+          <t>FMCC - PCKG 20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FLAGLER PL NW</t>
+          <t>QUEEN ST NE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -640,49 +640,49 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26065813</t>
+          <t xml:space="preserve"> 26063435</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>02/01/26 04:18 pm</t>
+          <t>01/30/26 08:43 am</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>02/05/26 07:00 am</t>
+          <t>02/04/26 08:45 am</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>02/24/26 07:00 am</t>
+          <t>02/23/26 08:45 am</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>COMDC - Not yet responded</t>
+          <t>COMDC, VDC, WASA02 &amp; WGL07 - Not yet responded &amp; DCDOT01 - Not complete/In progress</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>21 days, 17:23:45.788768</t>
+          <t>20 days, 14:25:50.886970</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EMERGENCY CREW ON SITE</t>
+          <t>FMCC - PCKG 20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4TH ST SE</t>
+          <t>N CAPITOL ST NW</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -697,54 +697,54 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26065582</t>
+          <t xml:space="preserve"> 26063418</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>01/31/26 06:03 pm</t>
+          <t>01/30/26 08:32 am</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>02/05/26 07:00 am</t>
+          <t>02/04/26 08:45 am</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>02/24/26 07:00 am</t>
+          <t>02/23/26 08:45 am</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>COMDC - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; QGS06, WASA02 &amp; WGL07 - Not yet responded</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>21 days, 17:23:45.788733</t>
+          <t>20 days, 14:25:50.886926</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EMERGENCY CREW EN ROUTE / ETA 9:30AM</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS FEB 05 &gt;&amp;...</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R ST NW</t>
+          <t>N CAPITOL ST NW</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Update-Renewal</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -754,54 +754,59 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26065458</t>
+          <t xml:space="preserve"> 26063400</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>26009812</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>01/31/26 08:34 am</t>
+          <t>01/30/26 08:28 am</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>02/05/26 07:00 am</t>
+          <t>02/03/26 08:30 am</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>02/24/26 07:00 am</t>
+          <t>02/23/26 08:30 am</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>COMDC - Not yet responded</t>
+          <t>WASA02 &amp; WGL07 - Not yet responded</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>21 days, 17:23:45.788703</t>
+          <t>20 days, 14:10:50.886882</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>QUEEN ST NE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Update-Renewal</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -811,54 +816,59 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26063435</t>
+          <t xml:space="preserve"> 26062791</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>26035381</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>01/30/26 08:43 am</t>
+          <t>01/29/26 03:50 pm</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>02/04/26 08:45 am</t>
+          <t>02/02/26 04:00 pm</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>02/23/26 08:45 am</t>
+          <t>02/20/26 04:00 pm</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>COMDC, VDC, WASA02 &amp; WGL07 - Not yet responded &amp; DCDOT01 - Not complete/In progress</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>20 days, 19:08:45.788658</t>
+          <t>17 days, 21:40:50.886839</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>N CAPITOL ST NW</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Update-Renewal</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -868,49 +878,54 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26063418</t>
+          <t xml:space="preserve"> 26062790</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>26035369</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>01/30/26 08:32 am</t>
+          <t>01/29/26 03:50 pm</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>02/04/26 08:45 am</t>
+          <t>02/02/26 04:00 pm</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>02/23/26 08:45 am</t>
+          <t>02/20/26 04:00 pm</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; QGS06, WASA02 &amp; WGL07 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>20 days, 19:08:45.788624</t>
+          <t>17 days, 21:40:50.886796</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS FEB 05 &gt;&amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N CAPITOL ST NW</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -925,42 +940,42 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26063400</t>
+          <t xml:space="preserve"> 26062789</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>26009812</t>
+          <t>26035377</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>01/30/26 08:28 am</t>
+          <t>01/29/26 03:50 pm</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>02/03/26 08:30 am</t>
+          <t>02/02/26 04:00 pm</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>02/23/26 08:30 am</t>
+          <t>02/20/26 04:00 pm</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>QGS06, WASA02 &amp; WGL07 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>20 days, 18:53:45.788593</t>
+          <t>17 days, 21:40:50.886753</t>
         </is>
       </c>
     </row>
@@ -987,12 +1002,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062791</t>
+          <t xml:space="preserve"> 26062788</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>26035381</t>
+          <t>26035371</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1012,24 +1027,24 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788554</t>
+          <t>17 days, 21:40:50.886714</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1049,12 +1064,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062790</t>
+          <t xml:space="preserve"> 26062787</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>26035369</t>
+          <t>26035379</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1074,17 +1089,17 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788520</t>
+          <t>17 days, 21:40:50.886675</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1126,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062789</t>
+          <t xml:space="preserve"> 26062786</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>26035377</t>
+          <t>26035382</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1136,17 +1151,17 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788471</t>
+          <t>17 days, 21:40:50.886629</t>
         </is>
       </c>
     </row>
@@ -1158,7 +1173,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>6TH ST SE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1173,12 +1188,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062788</t>
+          <t xml:space="preserve"> 26062785</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>26035371</t>
+          <t>26035365</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1198,17 +1213,17 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788440</t>
+          <t>17 days, 21:40:50.886587</t>
         </is>
       </c>
     </row>
@@ -1235,12 +1250,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062787</t>
+          <t xml:space="preserve"> 26062784</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>26035379</t>
+          <t>26035384</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1265,19 +1280,19 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788410</t>
+          <t>17 days, 21:40:50.886549</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1297,12 +1312,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062786</t>
+          <t xml:space="preserve"> 26062783</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>26035382</t>
+          <t>26035370</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1322,17 +1337,17 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788380</t>
+          <t>17 days, 21:40:50.886508</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1359,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6TH ST SE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1359,12 +1374,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062785</t>
+          <t xml:space="preserve"> 26062782</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>26035365</t>
+          <t>26035368</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1389,24 +1404,24 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788347</t>
+          <t>17 days, 21:40:50.886470</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>PCKG 20 UPDATE: WORK STARTS ON FEB 04 &gt;&gt;</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>7TH ST SE</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1421,12 +1436,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062784</t>
+          <t xml:space="preserve"> 26062781</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>26035384</t>
+          <t>26035387</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1446,29 +1461,29 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788317</t>
+          <t>17 days, 21:40:50.886434</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>6TH ST SE</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1483,12 +1498,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062783</t>
+          <t xml:space="preserve"> 26062780</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>26035370</t>
+          <t>26035362</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1513,12 +1528,12 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788285</t>
+          <t>17 days, 21:40:50.886394</t>
         </is>
       </c>
     </row>
@@ -1530,7 +1545,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>6TH ST SE</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1545,12 +1560,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062782</t>
+          <t xml:space="preserve"> 26062779</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>26035368</t>
+          <t>26035367</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1575,24 +1590,24 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788254</t>
+          <t>17 days, 21:40:50.886354</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PCKG 20 UPDATE: WORK STARTS ON FEB 04 &gt;&gt;</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7TH ST SE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1607,12 +1622,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062781</t>
+          <t xml:space="preserve"> 26062778</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>26035387</t>
+          <t>26035376</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1632,17 +1647,17 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788222</t>
+          <t>17 days, 21:40:50.886297</t>
         </is>
       </c>
     </row>
@@ -1669,12 +1684,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062780</t>
+          <t xml:space="preserve"> 26062777</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>26035362</t>
+          <t>26035373</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1694,17 +1709,17 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788190</t>
+          <t>17 days, 21:40:50.886257</t>
         </is>
       </c>
     </row>
@@ -1731,12 +1746,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062779</t>
+          <t xml:space="preserve"> 26062776</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>26035367</t>
+          <t>26035380</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1761,12 +1776,12 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788157</t>
+          <t>17 days, 21:40:50.886211</t>
         </is>
       </c>
     </row>
@@ -1793,12 +1808,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062778</t>
+          <t xml:space="preserve"> 26062775</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>26035376</t>
+          <t>26035372</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1823,12 +1838,12 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788127</t>
+          <t>17 days, 21:40:50.886174</t>
         </is>
       </c>
     </row>
@@ -1855,12 +1870,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062777</t>
+          <t xml:space="preserve"> 26062774</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>26035373</t>
+          <t>26035364</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1880,29 +1895,29 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788098</t>
+          <t>17 days, 21:40:50.886133</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6TH ST SE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1917,12 +1932,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062776</t>
+          <t xml:space="preserve"> 26062773</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>26035380</t>
+          <t>26035361</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1942,17 +1957,17 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788066</t>
+          <t>17 days, 21:40:50.886097</t>
         </is>
       </c>
     </row>
@@ -1979,12 +1994,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062775</t>
+          <t xml:space="preserve"> 26062772</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>26035372</t>
+          <t>26035366</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2009,24 +2024,24 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788036</t>
+          <t>17 days, 21:40:50.886061</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6TH ST SE</t>
+          <t>7TH ST SE</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2041,12 +2056,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062774</t>
+          <t xml:space="preserve"> 26062771</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>26035364</t>
+          <t>26035378</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2066,24 +2081,24 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.788003</t>
+          <t>17 days, 21:40:50.886022</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2103,12 +2118,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062773</t>
+          <t xml:space="preserve"> 26062770</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>26035361</t>
+          <t>26035375</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2128,17 +2143,17 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787973</t>
+          <t>17 days, 21:40:50.885985</t>
         </is>
       </c>
     </row>
@@ -2150,7 +2165,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>6TH ST SE</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2165,12 +2180,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062772</t>
+          <t xml:space="preserve"> 26062769</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>26035366</t>
+          <t>26035360</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2190,29 +2205,29 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787943</t>
+          <t>17 days, 21:40:50.885946</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7TH ST SE</t>
+          <t>6TH ST SE</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2227,12 +2242,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062771</t>
+          <t xml:space="preserve"> 26062768</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>26035378</t>
+          <t>26035386</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2252,24 +2267,24 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787912</t>
+          <t>17 days, 21:40:50.885908</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2289,12 +2304,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062770</t>
+          <t xml:space="preserve"> 26062767</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>26035375</t>
+          <t>26035363</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2314,17 +2329,17 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787883</t>
+          <t>17 days, 21:40:50.885873</t>
         </is>
       </c>
     </row>
@@ -2336,7 +2351,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6TH ST SE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2351,12 +2366,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062769</t>
+          <t xml:space="preserve"> 26062766</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>26035360</t>
+          <t>26035383</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2376,17 +2391,17 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787851</t>
+          <t>17 days, 21:40:50.885837</t>
         </is>
       </c>
     </row>
@@ -2398,7 +2413,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6TH ST SE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2413,12 +2428,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062768</t>
+          <t xml:space="preserve"> 26062765</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>26035386</t>
+          <t>26035374</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2443,19 +2458,19 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787820</t>
+          <t>17 days, 21:40:50.885797</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARTS ON FEB 04 &amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2475,12 +2490,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062767</t>
+          <t xml:space="preserve"> 26062764</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>26035363</t>
+          <t>26035385</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -2500,24 +2515,24 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787790</t>
+          <t>17 days, 21:40:50.885761</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&amp;...</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2537,17 +2552,17 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062766</t>
+          <t xml:space="preserve"> 26062763</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>26035383</t>
+          <t>26035393</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>01/29/26 03:50 pm</t>
+          <t>01/29/26 03:47 pm</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2562,29 +2577,29 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787760</t>
+          <t>17 days, 21:40:50.885724</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&gt;</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>6TH ST SE</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2599,17 +2614,17 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062765</t>
+          <t xml:space="preserve"> 26062762</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>26035374</t>
+          <t>26035399</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>01/29/26 03:50 pm</t>
+          <t>01/29/26 03:47 pm</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2624,29 +2639,29 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787729</t>
+          <t>17 days, 21:40:50.885688</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARTS ON FEB 04 ...</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&amp;...</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>7TH ST SE</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2661,17 +2676,17 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062764</t>
+          <t xml:space="preserve"> 26062761</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>26035385</t>
+          <t>26035408</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>01/29/26 03:50 pm</t>
+          <t>01/29/26 03:47 pm</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2686,24 +2701,24 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787699</t>
+          <t>17 days, 21:40:50.885653</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2723,12 +2738,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062763</t>
+          <t xml:space="preserve"> 26062760</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>26035393</t>
+          <t>26035405</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2748,24 +2763,24 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787669</t>
+          <t>17 days, 21:40:50.885616</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&gt;</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2785,12 +2800,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062762</t>
+          <t xml:space="preserve"> 26062759</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>26035399</t>
+          <t>26035390</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2810,29 +2825,29 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787640</t>
+          <t>17 days, 21:40:50.885577</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&amp;...</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7TH ST SE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2847,12 +2862,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062761</t>
+          <t xml:space="preserve"> 26062758</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>26035408</t>
+          <t>26035412</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2877,12 +2892,12 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787611</t>
+          <t>17 days, 21:40:50.885541</t>
         </is>
       </c>
     </row>
@@ -2909,12 +2924,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062760</t>
+          <t xml:space="preserve"> 26062757</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>26035405</t>
+          <t>26035388</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2934,17 +2949,17 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787582</t>
+          <t>17 days, 21:40:50.885505</t>
         </is>
       </c>
     </row>
@@ -2956,7 +2971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6TH ST SE</t>
+          <t>F STREET TER SE</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2971,12 +2986,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062759</t>
+          <t xml:space="preserve"> 26062756</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>26035390</t>
+          <t>26035401</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -3001,19 +3016,19 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787550</t>
+          <t>17 days, 21:40:50.885466</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
+          <t>PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&gt;</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3033,12 +3048,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062758</t>
+          <t xml:space="preserve"> 26062755</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>26035412</t>
+          <t>26035396</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -3058,17 +3073,17 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787521</t>
+          <t>17 days, 21:40:50.885427</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3110,12 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062757</t>
+          <t xml:space="preserve"> 26062754</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>26035388</t>
+          <t>26035392</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -3120,29 +3135,29 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
+          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787483</t>
+          <t>17 days, 21:40:50.885388</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
+          <t>FMCC- PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&amp;...</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>6TH ST SE</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3157,12 +3172,12 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062756</t>
+          <t xml:space="preserve"> 26062753</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>26035401</t>
+          <t>26035403</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -3187,19 +3202,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787451</t>
+          <t>17 days, 21:40:50.885351</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&gt;</t>
+          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3219,12 +3234,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062755</t>
+          <t xml:space="preserve"> 26062752</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>26035396</t>
+          <t>26035400</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -3244,17 +3259,17 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787420</t>
+          <t>17 days, 21:40:50.885299</t>
         </is>
       </c>
     </row>
@@ -3266,7 +3281,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>F STREET TER SE</t>
+          <t>7TH ST SE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3281,12 +3296,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26062754</t>
+          <t xml:space="preserve"> 26062751</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>26035392</t>
+          <t>26035406</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -3306,203 +3321,17 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
+          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>18 days, 2:23:45.787388</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>FMCC- PCKG 20 UPDATE: WORK STARS FEB 04 &gt;&amp;...</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>6TH ST SE</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Update-Renewal</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 26062753</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>26035403</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>01/29/26 03:47 pm</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>02/02/26 04:00 pm</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>02/20/26 04:00 pm</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>DCDOT01 - Not complete/In progress &amp; VDC &amp; WGL07 - 24-hour delay &amp; WASA02 - Not yet responded</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>18 days, 2:23:45.787356</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>F STREET TER SE</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Update-Renewal</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 26062752</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>26035400</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>01/29/26 03:47 pm</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>02/02/26 04:00 pm</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>02/20/26 04:00 pm</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>18 days, 2:23:45.787327</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>FMCC - PCKG 20 UPDATE: WORK STARS FEB 04 &gt;...</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>7TH ST SE</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Update-Renewal</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 26062751</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>26035406</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>01/29/26 03:47 pm</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>02/02/26 04:00 pm</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>02/20/26 04:00 pm</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>DCDOT01 - Not complete/In progress &amp; WASA02 - Not yet responded &amp; WGL07 - 24-hour delay</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>18 days, 2:23:45.787297</t>
+          <t>17 days, 21:40:50.885262</t>
         </is>
       </c>
     </row>

</xml_diff>